<commit_message>
Updating for the games on Jan22
</commit_message>
<xml_diff>
--- a/workingdata/error_predics.xlsx
+++ b/workingdata/error_predics.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericshannon/Documents/ncaa_predictions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericshannon/Documents/ncaa_predictions/workingdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1D281E-C54F-7A4B-9D4B-31063E74D73B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{613B7893-622B-7440-9E14-5D87AA1AF2BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11340" yWindow="480" windowWidth="12980" windowHeight="13300" activeTab="1" xr2:uid="{3631A22F-5DE8-4F4D-9E8A-2705B43EDF70}"/>
+    <workbookView xWindow="7900" yWindow="600" windowWidth="10000" windowHeight="13760" activeTab="2" xr2:uid="{3631A22F-5DE8-4F4D-9E8A-2705B43EDF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Jan19(61pct)" sheetId="1" r:id="rId1"/>
     <sheet name="Jan21(65pct)" sheetId="3" r:id="rId2"/>
+    <sheet name="Jan22(47pct)" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="324">
   <si>
     <t>Home</t>
   </si>
@@ -968,6 +969,36 @@
   </si>
   <si>
     <t>Marist</t>
+  </si>
+  <si>
+    <t>Clemson</t>
+  </si>
+  <si>
+    <t>Florida State</t>
+  </si>
+  <si>
+    <t>Villanova</t>
+  </si>
+  <si>
+    <t>Northwestern</t>
+  </si>
+  <si>
+    <t>Buffalo</t>
+  </si>
+  <si>
+    <t>Eastern Michigan</t>
+  </si>
+  <si>
+    <t>Toledo</t>
+  </si>
+  <si>
+    <t>Ohio</t>
+  </si>
+  <si>
+    <t>San Diego State</t>
+  </si>
+  <si>
+    <t>Saint Peter's</t>
   </si>
 </sst>
 </file>
@@ -3474,8 +3505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1976368E-125D-E94E-93E9-C65104DE4812}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3949,4 +3980,359 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EDF4423-1E55-024A-85E0-88E05E41E0B0}">
+  <dimension ref="A1:D24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2">
+        <v>41</v>
+      </c>
+      <c r="D2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3">
+        <v>79</v>
+      </c>
+      <c r="D3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4">
+        <v>45</v>
+      </c>
+      <c r="D4">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>314</v>
+      </c>
+      <c r="B5" t="s">
+        <v>315</v>
+      </c>
+      <c r="C5">
+        <v>68</v>
+      </c>
+      <c r="D5">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6">
+        <v>61</v>
+      </c>
+      <c r="D6">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7">
+        <v>45</v>
+      </c>
+      <c r="D7">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>316</v>
+      </c>
+      <c r="B8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8">
+        <v>80</v>
+      </c>
+      <c r="D8">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9">
+        <v>57</v>
+      </c>
+      <c r="D9">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" t="s">
+        <v>317</v>
+      </c>
+      <c r="C10">
+        <v>66</v>
+      </c>
+      <c r="D10">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>318</v>
+      </c>
+      <c r="B11" t="s">
+        <v>147</v>
+      </c>
+      <c r="C11">
+        <v>75</v>
+      </c>
+      <c r="D11">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>150</v>
+      </c>
+      <c r="B12" t="s">
+        <v>143</v>
+      </c>
+      <c r="C12">
+        <v>67</v>
+      </c>
+      <c r="D12">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>144</v>
+      </c>
+      <c r="B13" t="s">
+        <v>149</v>
+      </c>
+      <c r="C13">
+        <v>71</v>
+      </c>
+      <c r="D13">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>146</v>
+      </c>
+      <c r="B14" t="s">
+        <v>319</v>
+      </c>
+      <c r="C14">
+        <v>80</v>
+      </c>
+      <c r="D14">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>320</v>
+      </c>
+      <c r="B15" t="s">
+        <v>145</v>
+      </c>
+      <c r="C15">
+        <v>85</v>
+      </c>
+      <c r="D15">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>148</v>
+      </c>
+      <c r="B16" t="s">
+        <v>321</v>
+      </c>
+      <c r="C16">
+        <v>76</v>
+      </c>
+      <c r="D16">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>166</v>
+      </c>
+      <c r="B17" t="s">
+        <v>163</v>
+      </c>
+      <c r="C17">
+        <v>60</v>
+      </c>
+      <c r="D17">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>168</v>
+      </c>
+      <c r="B18" t="s">
+        <v>170</v>
+      </c>
+      <c r="C18">
+        <v>58</v>
+      </c>
+      <c r="D18">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>322</v>
+      </c>
+      <c r="B19" t="s">
+        <v>165</v>
+      </c>
+      <c r="C19">
+        <v>62</v>
+      </c>
+      <c r="D19">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>323</v>
+      </c>
+      <c r="B20" t="s">
+        <v>141</v>
+      </c>
+      <c r="C20">
+        <v>74</v>
+      </c>
+      <c r="D20">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>227</v>
+      </c>
+      <c r="B21" t="s">
+        <v>223</v>
+      </c>
+      <c r="C21">
+        <v>55</v>
+      </c>
+      <c r="D21">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>224</v>
+      </c>
+      <c r="B22" t="s">
+        <v>233</v>
+      </c>
+      <c r="C22">
+        <v>77</v>
+      </c>
+      <c r="D22">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>226</v>
+      </c>
+      <c r="B23" t="s">
+        <v>221</v>
+      </c>
+      <c r="C23">
+        <v>53</v>
+      </c>
+      <c r="D23">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>232</v>
+      </c>
+      <c r="B24" t="s">
+        <v>229</v>
+      </c>
+      <c r="C24">
+        <v>72</v>
+      </c>
+      <c r="D24">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updating with game results for 20190123
</commit_message>
<xml_diff>
--- a/workingdata/error_predics.xlsx
+++ b/workingdata/error_predics.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericshannon/Documents/ncaa_predictions/workingdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{613B7893-622B-7440-9E14-5D87AA1AF2BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA24179-E44F-BD4C-8145-CE780AADA752}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7900" yWindow="600" windowWidth="10000" windowHeight="13760" activeTab="2" xr2:uid="{3631A22F-5DE8-4F4D-9E8A-2705B43EDF70}"/>
+    <workbookView xWindow="7320" yWindow="1320" windowWidth="10000" windowHeight="13760" firstSheet="1" activeTab="3" xr2:uid="{3631A22F-5DE8-4F4D-9E8A-2705B43EDF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Jan19(61pct)" sheetId="1" r:id="rId1"/>
     <sheet name="Jan21(65pct)" sheetId="3" r:id="rId2"/>
     <sheet name="Jan22(47pct)" sheetId="4" r:id="rId3"/>
+    <sheet name="Jan23" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="342">
   <si>
     <t>Home</t>
   </si>
@@ -999,6 +1000,60 @@
   </si>
   <si>
     <t>Saint Peter's</t>
+  </si>
+  <si>
+    <t>East Carolina</t>
+  </si>
+  <si>
+    <t>New Hampshire</t>
+  </si>
+  <si>
+    <t>George Washington</t>
+  </si>
+  <si>
+    <t>Saint Joseph's</t>
+  </si>
+  <si>
+    <t>Saint Louis</t>
+  </si>
+  <si>
+    <t>Duquesne</t>
+  </si>
+  <si>
+    <t>Maquette</t>
+  </si>
+  <si>
+    <t>Providence</t>
+  </si>
+  <si>
+    <t>Xavier</t>
+  </si>
+  <si>
+    <t>Ohio State</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t>Bradley</t>
+  </si>
+  <si>
+    <t>Drake</t>
+  </si>
+  <si>
+    <t>Southern Illinois</t>
+  </si>
+  <si>
+    <t>Missouri State</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Lamar</t>
+  </si>
+  <si>
+    <t>South Dakota</t>
   </si>
 </sst>
 </file>
@@ -3986,8 +4041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EDF4423-1E55-024A-85E0-88E05E41E0B0}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4335,4 +4390,653 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A6C6588-F104-0540-BED5-75CB2F72467E}">
+  <dimension ref="A1:D45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+      <c r="D2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3">
+        <v>75</v>
+      </c>
+      <c r="D3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4">
+        <v>67</v>
+      </c>
+      <c r="D4">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5">
+        <v>85</v>
+      </c>
+      <c r="D5">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>325</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6">
+        <v>39</v>
+      </c>
+      <c r="D6">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7">
+        <v>74</v>
+      </c>
+      <c r="D7">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>326</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>62</v>
+      </c>
+      <c r="D8">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>67</v>
+      </c>
+      <c r="D9">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>73</v>
+      </c>
+      <c r="D10">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <v>65</v>
+      </c>
+      <c r="D11">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <v>65</v>
+      </c>
+      <c r="D12">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>327</v>
+      </c>
+      <c r="C13">
+        <v>70</v>
+      </c>
+      <c r="D13">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>328</v>
+      </c>
+      <c r="B14" t="s">
+        <v>329</v>
+      </c>
+      <c r="C14">
+        <v>73</v>
+      </c>
+      <c r="D14">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15">
+        <v>61</v>
+      </c>
+      <c r="D15">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16">
+        <v>70</v>
+      </c>
+      <c r="D16">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" t="s">
+        <v>330</v>
+      </c>
+      <c r="C17">
+        <v>69</v>
+      </c>
+      <c r="D17">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>331</v>
+      </c>
+      <c r="B18" t="s">
+        <v>332</v>
+      </c>
+      <c r="C18">
+        <v>64</v>
+      </c>
+      <c r="D18">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" t="s">
+        <v>333</v>
+      </c>
+      <c r="C19">
+        <v>79</v>
+      </c>
+      <c r="D19">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" t="s">
+        <v>334</v>
+      </c>
+      <c r="C20">
+        <v>72</v>
+      </c>
+      <c r="D20">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" t="s">
+        <v>93</v>
+      </c>
+      <c r="C21">
+        <v>71</v>
+      </c>
+      <c r="D21">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22">
+        <v>74</v>
+      </c>
+      <c r="D22">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23">
+        <v>75</v>
+      </c>
+      <c r="D23">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24" t="s">
+        <v>299</v>
+      </c>
+      <c r="C24">
+        <v>78</v>
+      </c>
+      <c r="D24">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>169</v>
+      </c>
+      <c r="B25" t="s">
+        <v>167</v>
+      </c>
+      <c r="C25">
+        <v>46</v>
+      </c>
+      <c r="D25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>173</v>
+      </c>
+      <c r="B26" t="s">
+        <v>335</v>
+      </c>
+      <c r="C26">
+        <v>68</v>
+      </c>
+      <c r="D26">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>178</v>
+      </c>
+      <c r="B27" t="s">
+        <v>176</v>
+      </c>
+      <c r="C27">
+        <v>53</v>
+      </c>
+      <c r="D27">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>174</v>
+      </c>
+      <c r="B28" t="s">
+        <v>336</v>
+      </c>
+      <c r="C28">
+        <v>66</v>
+      </c>
+      <c r="D28">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>177</v>
+      </c>
+      <c r="B29" t="s">
+        <v>337</v>
+      </c>
+      <c r="C29">
+        <v>62</v>
+      </c>
+      <c r="D29">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>175</v>
+      </c>
+      <c r="B30" t="s">
+        <v>338</v>
+      </c>
+      <c r="C30">
+        <v>35</v>
+      </c>
+      <c r="D30">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>218</v>
+      </c>
+      <c r="B31" t="s">
+        <v>216</v>
+      </c>
+      <c r="C31">
+        <v>70</v>
+      </c>
+      <c r="D31">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>214</v>
+      </c>
+      <c r="B32" t="s">
+        <v>220</v>
+      </c>
+      <c r="C32">
+        <v>57</v>
+      </c>
+      <c r="D32">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>213</v>
+      </c>
+      <c r="B33" t="s">
+        <v>211</v>
+      </c>
+      <c r="C33">
+        <v>68</v>
+      </c>
+      <c r="D33">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>217</v>
+      </c>
+      <c r="B34" t="s">
+        <v>215</v>
+      </c>
+      <c r="C34">
+        <v>47</v>
+      </c>
+      <c r="D34">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>212</v>
+      </c>
+      <c r="B35" t="s">
+        <v>219</v>
+      </c>
+      <c r="C35">
+        <v>85</v>
+      </c>
+      <c r="D35">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>222</v>
+      </c>
+      <c r="B36" t="s">
+        <v>228</v>
+      </c>
+      <c r="C36">
+        <v>88</v>
+      </c>
+      <c r="D36">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>339</v>
+      </c>
+      <c r="B37" t="s">
+        <v>234</v>
+      </c>
+      <c r="C37">
+        <v>82</v>
+      </c>
+      <c r="D37">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>231</v>
+      </c>
+      <c r="B38" t="s">
+        <v>225</v>
+      </c>
+      <c r="C38">
+        <v>60</v>
+      </c>
+      <c r="D38">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>264</v>
+      </c>
+      <c r="B39" t="s">
+        <v>262</v>
+      </c>
+      <c r="C39">
+        <v>78</v>
+      </c>
+      <c r="D39">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>263</v>
+      </c>
+      <c r="B40" t="s">
+        <v>256</v>
+      </c>
+      <c r="C40">
+        <v>60</v>
+      </c>
+      <c r="D40">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>260</v>
+      </c>
+      <c r="B41" t="s">
+        <v>259</v>
+      </c>
+      <c r="C41">
+        <v>71</v>
+      </c>
+      <c r="D41">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>255</v>
+      </c>
+      <c r="B42" t="s">
+        <v>265</v>
+      </c>
+      <c r="C42">
+        <v>70</v>
+      </c>
+      <c r="D42">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>257</v>
+      </c>
+      <c r="B43" t="s">
+        <v>340</v>
+      </c>
+      <c r="C43">
+        <v>81</v>
+      </c>
+      <c r="D43">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>258</v>
+      </c>
+      <c r="B44" t="s">
+        <v>261</v>
+      </c>
+      <c r="C44">
+        <v>73</v>
+      </c>
+      <c r="D44">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>341</v>
+      </c>
+      <c r="B45" t="s">
+        <v>266</v>
+      </c>
+      <c r="C45">
+        <v>70</v>
+      </c>
+      <c r="D45">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>